<commit_message>
ok can change password
</commit_message>
<xml_diff>
--- a/data/user.xlsx
+++ b/data/user.xlsx
@@ -464,8 +464,10 @@
           <t>admin</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>19373469</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -492,10 +494,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>

</xml_diff>